<commit_message>
update the polarity catagories
</commit_message>
<xml_diff>
--- a/Polarity_Segment.xlsx
+++ b/Polarity_Segment.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="816">
   <si>
     <t>LineCode</t>
   </si>
@@ -2469,13 +2469,16 @@
   </si>
   <si>
     <t>1B1</t>
+  </si>
+  <si>
+    <t>JRC_SS03799-20151014_32_F1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -2487,6 +2490,22 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2509,8 +2528,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2531,7 +2556,13 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2861,10 +2892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D581"/>
+  <dimension ref="A1:D582"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="300" zoomScaleNormal="300" zoomScalePageLayoutView="300" workbookViewId="0">
-      <selection activeCell="D141" sqref="D141"/>
+    <sheetView tabSelected="1" topLeftCell="A254" zoomScale="300" zoomScaleNormal="300" zoomScalePageLayoutView="300" workbookViewId="0">
+      <selection activeCell="C265" sqref="C265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6569,13 +6600,13 @@
       </c>
     </row>
     <row r="265" spans="1:4">
-      <c r="A265" s="2" t="s">
+      <c r="A265" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B265" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="C265" s="4" t="s">
+      <c r="B265" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="C265" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D265" s="5" t="s">
@@ -6584,44 +6615,44 @@
     </row>
     <row r="266" spans="1:4">
       <c r="A266" s="2" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C266" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D266" s="5" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
     </row>
     <row r="267" spans="1:4">
       <c r="A267" s="2" t="s">
-        <v>239</v>
+        <v>171</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C267" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D267" s="5" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
     </row>
     <row r="268" spans="1:4">
       <c r="A268" s="2" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C268" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D268" s="5" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -6629,7 +6660,7 @@
         <v>180</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C269" s="4" t="s">
         <v>6</v>
@@ -6640,16 +6671,16 @@
     </row>
     <row r="270" spans="1:4">
       <c r="A270" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D270" s="5" t="s">
-        <v>814</v>
+        <v>10</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -6657,7 +6688,7 @@
         <v>183</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>6</v>
@@ -6671,7 +6702,7 @@
         <v>183</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>6</v>
@@ -6685,7 +6716,7 @@
         <v>183</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C273" s="4" t="s">
         <v>6</v>
@@ -6696,30 +6727,30 @@
     </row>
     <row r="274" spans="1:4">
       <c r="A274" s="2" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C274" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D274" s="5" t="s">
-        <v>41</v>
+        <v>814</v>
       </c>
     </row>
     <row r="275" spans="1:4">
       <c r="A275" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C275" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D275" s="5" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -6727,7 +6758,7 @@
         <v>204</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C276" s="4" t="s">
         <v>6</v>
@@ -6741,7 +6772,7 @@
         <v>204</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C277" s="4" t="s">
         <v>6</v>
@@ -6752,16 +6783,16 @@
     </row>
     <row r="278" spans="1:4">
       <c r="A278" s="2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C278" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D278" s="5" t="s">
-        <v>217</v>
+        <v>26</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -6769,7 +6800,7 @@
         <v>215</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C279" s="4" t="s">
         <v>6</v>
@@ -6783,7 +6814,7 @@
         <v>215</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C280" s="4" t="s">
         <v>6</v>
@@ -6794,16 +6825,16 @@
     </row>
     <row r="281" spans="1:4">
       <c r="A281" s="2" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C281" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D281" s="5" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -6811,7 +6842,7 @@
         <v>227</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C282" s="4" t="s">
         <v>6</v>
@@ -6822,16 +6853,16 @@
     </row>
     <row r="283" spans="1:4">
       <c r="A283" s="2" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C283" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D283" s="5" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -6839,7 +6870,7 @@
         <v>242</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C284" s="4" t="s">
         <v>6</v>
@@ -6853,7 +6884,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C285" s="4" t="s">
         <v>6</v>
@@ -6867,7 +6898,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C286" s="4" t="s">
         <v>6</v>
@@ -6881,7 +6912,7 @@
         <v>242</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C287" s="4" t="s">
         <v>6</v>
@@ -6895,7 +6926,7 @@
         <v>242</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C288" s="4" t="s">
         <v>6</v>
@@ -6906,30 +6937,30 @@
     </row>
     <row r="289" spans="1:4">
       <c r="A289" s="2" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C289" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D289" s="5" t="s">
-        <v>54</v>
+        <v>244</v>
       </c>
     </row>
     <row r="290" spans="1:4">
       <c r="A290" s="2" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C290" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D290" s="5" t="s">
-        <v>278</v>
+        <v>54</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -6937,7 +6968,7 @@
         <v>276</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C291" s="4" t="s">
         <v>6</v>
@@ -6951,7 +6982,7 @@
         <v>276</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C292" s="4" t="s">
         <v>6</v>
@@ -6965,7 +6996,7 @@
         <v>276</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C293" s="4" t="s">
         <v>6</v>
@@ -6976,16 +7007,16 @@
     </row>
     <row r="294" spans="1:4">
       <c r="A294" s="2" t="s">
-        <v>429</v>
+        <v>276</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C294" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D294" s="5" t="s">
-        <v>73</v>
+        <v>278</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -6993,7 +7024,7 @@
         <v>429</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C295" s="4" t="s">
         <v>6</v>
@@ -7004,16 +7035,16 @@
     </row>
     <row r="296" spans="1:4">
       <c r="A296" s="2" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C296" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D296" s="5" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -7021,7 +7052,7 @@
         <v>432</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C297" s="4" t="s">
         <v>6</v>
@@ -7035,7 +7066,7 @@
         <v>432</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C298" s="4" t="s">
         <v>6</v>
@@ -7049,7 +7080,7 @@
         <v>432</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C299" s="4" t="s">
         <v>6</v>
@@ -7063,7 +7094,7 @@
         <v>432</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C300" s="4" t="s">
         <v>6</v>
@@ -7074,16 +7105,16 @@
     </row>
     <row r="301" spans="1:4">
       <c r="A301" s="2" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C301" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D301" s="5" t="s">
-        <v>440</v>
+        <v>225</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -7091,7 +7122,7 @@
         <v>438</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C302" s="4" t="s">
         <v>6</v>
@@ -7105,7 +7136,7 @@
         <v>438</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C303" s="4" t="s">
         <v>6</v>
@@ -7116,16 +7147,16 @@
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="2" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C304" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D304" s="5" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -7133,7 +7164,7 @@
         <v>443</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C305" s="4" t="s">
         <v>6</v>
@@ -7147,7 +7178,7 @@
         <v>443</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C306" s="4" t="s">
         <v>6</v>
@@ -7158,30 +7189,30 @@
     </row>
     <row r="307" spans="1:4">
       <c r="A307" s="2" t="s">
-        <v>288</v>
+        <v>443</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C307" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D307" s="5" t="s">
-        <v>290</v>
+        <v>445</v>
       </c>
     </row>
     <row r="308" spans="1:4">
       <c r="A308" s="2" t="s">
-        <v>449</v>
+        <v>288</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C308" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D308" s="5" t="s">
-        <v>13</v>
+        <v>290</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -7189,7 +7220,7 @@
         <v>449</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C309" s="4" t="s">
         <v>6</v>
@@ -7203,7 +7234,7 @@
         <v>449</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C310" s="4" t="s">
         <v>6</v>
@@ -7214,30 +7245,30 @@
     </row>
     <row r="311" spans="1:4">
       <c r="A311" s="2" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C311" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D311" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="312" spans="1:4">
       <c r="A312" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C312" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D312" s="5" t="s">
-        <v>457</v>
+        <v>35</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -7245,7 +7276,7 @@
         <v>455</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C313" s="4" t="s">
         <v>6</v>
@@ -7259,7 +7290,7 @@
         <v>455</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C314" s="4" t="s">
         <v>6</v>
@@ -7273,7 +7304,7 @@
         <v>455</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C315" s="4" t="s">
         <v>6</v>
@@ -7287,7 +7318,7 @@
         <v>455</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C316" s="4" t="s">
         <v>6</v>
@@ -7298,30 +7329,30 @@
     </row>
     <row r="317" spans="1:4">
       <c r="A317" s="2" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C317" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D317" s="5" t="s">
-        <v>22</v>
+        <v>457</v>
       </c>
     </row>
     <row r="318" spans="1:4">
       <c r="A318" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C318" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D318" s="5" t="s">
-        <v>466</v>
+        <v>22</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -7329,7 +7360,7 @@
         <v>464</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C319" s="4" t="s">
         <v>6</v>
@@ -7343,7 +7374,7 @@
         <v>464</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C320" s="4" t="s">
         <v>6</v>
@@ -7357,7 +7388,7 @@
         <v>464</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C321" s="4" t="s">
         <v>6</v>
@@ -7371,7 +7402,7 @@
         <v>464</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C322" s="4" t="s">
         <v>6</v>
@@ -7385,7 +7416,7 @@
         <v>464</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C323" s="4" t="s">
         <v>6</v>
@@ -7396,30 +7427,30 @@
     </row>
     <row r="324" spans="1:4">
       <c r="A324" s="2" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C324" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D324" s="5" t="s">
-        <v>73</v>
+        <v>466</v>
       </c>
     </row>
     <row r="325" spans="1:4">
       <c r="A325" s="2" t="s">
-        <v>44</v>
+        <v>472</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C325" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D325" s="5" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -7427,7 +7458,7 @@
         <v>44</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C326" s="4" t="s">
         <v>6</v>
@@ -7441,7 +7472,7 @@
         <v>44</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C327" s="4" t="s">
         <v>6</v>
@@ -7455,7 +7486,7 @@
         <v>44</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C328" s="4" t="s">
         <v>6</v>
@@ -7469,7 +7500,7 @@
         <v>44</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C329" s="4" t="s">
         <v>6</v>
@@ -7483,7 +7514,7 @@
         <v>44</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C330" s="4" t="s">
         <v>6</v>
@@ -7497,7 +7528,7 @@
         <v>44</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C331" s="4" t="s">
         <v>6</v>
@@ -7511,7 +7542,7 @@
         <v>44</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C332" s="4" t="s">
         <v>6</v>
@@ -7522,16 +7553,16 @@
     </row>
     <row r="333" spans="1:4">
       <c r="A333" s="2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C333" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D333" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -7539,7 +7570,7 @@
         <v>16</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C334" s="4" t="s">
         <v>6</v>
@@ -7553,7 +7584,7 @@
         <v>16</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C335" s="4" t="s">
         <v>6</v>
@@ -7567,7 +7598,7 @@
         <v>16</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C336" s="4" t="s">
         <v>6</v>
@@ -7581,7 +7612,7 @@
         <v>16</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C337" s="4" t="s">
         <v>6</v>
@@ -7595,7 +7626,7 @@
         <v>16</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C338" s="4" t="s">
         <v>6</v>
@@ -7609,7 +7640,7 @@
         <v>16</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C339" s="4" t="s">
         <v>6</v>
@@ -7623,7 +7654,7 @@
         <v>16</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C340" s="4" t="s">
         <v>6</v>
@@ -7634,16 +7665,16 @@
     </row>
     <row r="341" spans="1:4">
       <c r="A341" s="2" t="s">
-        <v>490</v>
+        <v>16</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C341" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D341" s="5" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -7651,7 +7682,7 @@
         <v>490</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C342" s="4" t="s">
         <v>6</v>
@@ -7662,16 +7693,16 @@
     </row>
     <row r="343" spans="1:4">
       <c r="A343" s="2" t="s">
-        <v>64</v>
+        <v>490</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C343" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D343" s="5" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -7679,7 +7710,7 @@
         <v>64</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C344" s="4" t="s">
         <v>6</v>
@@ -7693,7 +7724,7 @@
         <v>64</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C345" s="4" t="s">
         <v>6</v>
@@ -7707,7 +7738,7 @@
         <v>64</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C346" s="4" t="s">
         <v>6</v>
@@ -7718,16 +7749,16 @@
     </row>
     <row r="347" spans="1:4">
       <c r="A347" s="2" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C347" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D347" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -7735,7 +7766,7 @@
         <v>33</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C348" s="4" t="s">
         <v>6</v>
@@ -7749,7 +7780,7 @@
         <v>33</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C349" s="4" t="s">
         <v>6</v>
@@ -7763,7 +7794,7 @@
         <v>33</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C350" s="4" t="s">
         <v>6</v>
@@ -7774,16 +7805,16 @@
     </row>
     <row r="351" spans="1:4">
       <c r="A351" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C351" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D351" s="5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -7791,7 +7822,7 @@
         <v>24</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C352" s="4" t="s">
         <v>6</v>
@@ -7802,16 +7833,16 @@
     </row>
     <row r="353" spans="1:4">
       <c r="A353" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C353" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D353" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -7819,7 +7850,7 @@
         <v>20</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C354" s="4" t="s">
         <v>6</v>
@@ -7833,7 +7864,7 @@
         <v>20</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C355" s="4" t="s">
         <v>6</v>
@@ -7847,7 +7878,7 @@
         <v>20</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C356" s="4" t="s">
         <v>6</v>
@@ -7858,44 +7889,44 @@
     </row>
     <row r="357" spans="1:4">
       <c r="A357" s="2" t="s">
-        <v>297</v>
+        <v>20</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C357" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D357" s="5" t="s">
-        <v>299</v>
+        <v>22</v>
       </c>
     </row>
     <row r="358" spans="1:4">
       <c r="A358" s="2" t="s">
-        <v>508</v>
+        <v>297</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C358" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D358" s="5" t="s">
-        <v>10</v>
+        <v>299</v>
       </c>
     </row>
     <row r="359" spans="1:4">
       <c r="A359" s="2" t="s">
-        <v>310</v>
+        <v>508</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C359" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D359" s="5" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -7903,7 +7934,7 @@
         <v>310</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C360" s="4" t="s">
         <v>6</v>
@@ -7917,7 +7948,7 @@
         <v>310</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C361" s="4" t="s">
         <v>6</v>
@@ -7931,7 +7962,7 @@
         <v>310</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C362" s="4" t="s">
         <v>6</v>
@@ -7945,7 +7976,7 @@
         <v>310</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C363" s="4" t="s">
         <v>6</v>
@@ -7959,7 +7990,7 @@
         <v>310</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C364" s="4" t="s">
         <v>6</v>
@@ -7970,16 +8001,16 @@
     </row>
     <row r="365" spans="1:4">
       <c r="A365" s="2" t="s">
-        <v>516</v>
+        <v>310</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C365" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D365" s="5" t="s">
-        <v>229</v>
+        <v>54</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -7987,7 +8018,7 @@
         <v>516</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C366" s="4" t="s">
         <v>6</v>
@@ -8001,7 +8032,7 @@
         <v>516</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C367" s="4" t="s">
         <v>6</v>
@@ -8015,7 +8046,7 @@
         <v>516</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C368" s="4" t="s">
         <v>6</v>
@@ -8029,7 +8060,7 @@
         <v>516</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C369" s="4" t="s">
         <v>6</v>
@@ -8043,7 +8074,7 @@
         <v>516</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C370" s="4" t="s">
         <v>6</v>
@@ -8054,16 +8085,16 @@
     </row>
     <row r="371" spans="1:4">
       <c r="A371" s="2" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C371" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D371" s="5" t="s">
-        <v>54</v>
+        <v>229</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -8071,7 +8102,7 @@
         <v>523</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C372" s="4" t="s">
         <v>6</v>
@@ -8085,7 +8116,7 @@
         <v>523</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C373" s="4" t="s">
         <v>6</v>
@@ -8096,16 +8127,16 @@
     </row>
     <row r="374" spans="1:4">
       <c r="A374" s="2" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C374" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D374" s="5" t="s">
-        <v>173</v>
+        <v>54</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -8113,7 +8144,7 @@
         <v>527</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C375" s="4" t="s">
         <v>6</v>
@@ -8127,7 +8158,7 @@
         <v>527</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C376" s="4" t="s">
         <v>6</v>
@@ -8141,7 +8172,7 @@
         <v>527</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C377" s="4" t="s">
         <v>6</v>
@@ -8155,7 +8186,7 @@
         <v>527</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C378" s="4" t="s">
         <v>6</v>
@@ -8166,16 +8197,16 @@
     </row>
     <row r="379" spans="1:4">
       <c r="A379" s="2" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C379" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D379" s="5" t="s">
-        <v>466</v>
+        <v>173</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -8183,7 +8214,7 @@
         <v>533</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C380" s="4" t="s">
         <v>6</v>
@@ -8194,16 +8225,16 @@
     </row>
     <row r="381" spans="1:4">
       <c r="A381" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C381" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D381" s="5" t="s">
-        <v>538</v>
+        <v>466</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -8211,7 +8242,7 @@
         <v>536</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C382" s="4" t="s">
         <v>6</v>
@@ -8225,7 +8256,7 @@
         <v>536</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C383" s="4" t="s">
         <v>6</v>
@@ -8236,16 +8267,16 @@
     </row>
     <row r="384" spans="1:4">
       <c r="A384" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C384" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D384" s="5" t="s">
-        <v>814</v>
+        <v>538</v>
       </c>
     </row>
     <row r="385" spans="1:4">
@@ -8253,7 +8284,7 @@
         <v>541</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C385" s="4" t="s">
         <v>6</v>
@@ -8267,7 +8298,7 @@
         <v>541</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C386" s="4" t="s">
         <v>6</v>
@@ -8281,7 +8312,7 @@
         <v>541</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C387" s="4" t="s">
         <v>6</v>
@@ -8295,7 +8326,7 @@
         <v>541</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C388" s="4" t="s">
         <v>6</v>
@@ -8306,16 +8337,16 @@
     </row>
     <row r="389" spans="1:4">
       <c r="A389" s="2" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C389" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D389" s="5" t="s">
-        <v>26</v>
+        <v>814</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -8323,7 +8354,7 @@
         <v>547</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C390" s="4" t="s">
         <v>6</v>
@@ -8337,7 +8368,7 @@
         <v>547</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C391" s="4" t="s">
         <v>6</v>
@@ -8351,7 +8382,7 @@
         <v>547</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C392" s="4" t="s">
         <v>6</v>
@@ -8365,7 +8396,7 @@
         <v>547</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C393" s="4" t="s">
         <v>6</v>
@@ -8376,16 +8407,16 @@
     </row>
     <row r="394" spans="1:4">
       <c r="A394" s="2" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C394" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D394" s="5" t="s">
-        <v>555</v>
+        <v>26</v>
       </c>
     </row>
     <row r="395" spans="1:4">
@@ -8393,7 +8424,7 @@
         <v>553</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C395" s="4" t="s">
         <v>6</v>
@@ -8407,7 +8438,7 @@
         <v>553</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C396" s="4" t="s">
         <v>6</v>
@@ -8418,16 +8449,16 @@
     </row>
     <row r="397" spans="1:4">
       <c r="A397" s="2" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C397" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D397" s="5" t="s">
-        <v>125</v>
+        <v>555</v>
       </c>
     </row>
     <row r="398" spans="1:4">
@@ -8435,7 +8466,7 @@
         <v>558</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C398" s="4" t="s">
         <v>6</v>
@@ -8449,7 +8480,7 @@
         <v>558</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C399" s="4" t="s">
         <v>6</v>
@@ -8460,16 +8491,16 @@
     </row>
     <row r="400" spans="1:4">
       <c r="A400" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C400" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D400" s="5" t="s">
-        <v>564</v>
+        <v>125</v>
       </c>
     </row>
     <row r="401" spans="1:4">
@@ -8477,7 +8508,7 @@
         <v>562</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C401" s="4" t="s">
         <v>6</v>
@@ -8491,7 +8522,7 @@
         <v>562</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C402" s="4" t="s">
         <v>6</v>
@@ -8502,16 +8533,16 @@
     </row>
     <row r="403" spans="1:4">
       <c r="A403" s="2" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C403" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D403" s="5" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -8519,7 +8550,7 @@
         <v>567</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C404" s="4" t="s">
         <v>6</v>
@@ -8533,7 +8564,7 @@
         <v>567</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C405" s="4" t="s">
         <v>6</v>
@@ -8547,7 +8578,7 @@
         <v>567</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C406" s="4" t="s">
         <v>6</v>
@@ -8561,7 +8592,7 @@
         <v>567</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C407" s="4" t="s">
         <v>6</v>
@@ -8575,7 +8606,7 @@
         <v>567</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C408" s="4" t="s">
         <v>6</v>
@@ -8586,16 +8617,16 @@
     </row>
     <row r="409" spans="1:4">
       <c r="A409" s="2" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C409" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D409" s="5" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
     </row>
     <row r="410" spans="1:4">
@@ -8603,7 +8634,7 @@
         <v>575</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C410" s="4" t="s">
         <v>6</v>
@@ -8617,7 +8648,7 @@
         <v>575</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C411" s="4" t="s">
         <v>6</v>
@@ -8631,7 +8662,7 @@
         <v>575</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C412" s="4" t="s">
         <v>6</v>
@@ -8645,7 +8676,7 @@
         <v>575</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C413" s="4" t="s">
         <v>6</v>
@@ -8656,16 +8687,16 @@
     </row>
     <row r="414" spans="1:4">
       <c r="A414" s="2" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C414" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D414" s="5" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
     </row>
     <row r="415" spans="1:4">
@@ -8673,7 +8704,7 @@
         <v>582</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C415" s="4" t="s">
         <v>6</v>
@@ -8687,7 +8718,7 @@
         <v>582</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C416" s="4" t="s">
         <v>6</v>
@@ -8698,16 +8729,16 @@
     </row>
     <row r="417" spans="1:4">
       <c r="A417" s="2" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C417" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D417" s="5" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="418" spans="1:4">
@@ -8715,7 +8746,7 @@
         <v>587</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C418" s="4" t="s">
         <v>6</v>
@@ -8729,7 +8760,7 @@
         <v>587</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C419" s="4" t="s">
         <v>6</v>
@@ -8740,10 +8771,10 @@
     </row>
     <row r="420" spans="1:4">
       <c r="A420" s="2" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C420" s="4" t="s">
         <v>6</v>
@@ -8754,16 +8785,16 @@
     </row>
     <row r="421" spans="1:4">
       <c r="A421" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C421" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D421" s="5" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
     </row>
     <row r="422" spans="1:4">
@@ -8771,7 +8802,7 @@
         <v>594</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C422" s="4" t="s">
         <v>6</v>
@@ -8785,7 +8816,7 @@
         <v>594</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C423" s="4" t="s">
         <v>6</v>
@@ -8799,7 +8830,7 @@
         <v>594</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C424" s="4" t="s">
         <v>6</v>
@@ -8813,7 +8844,7 @@
         <v>594</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C425" s="4" t="s">
         <v>6</v>
@@ -8824,30 +8855,30 @@
     </row>
     <row r="426" spans="1:4">
       <c r="A426" s="2" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C426" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D426" s="5" t="s">
-        <v>602</v>
+        <v>584</v>
       </c>
     </row>
     <row r="427" spans="1:4">
       <c r="A427" s="2" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C427" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D427" s="5" t="s">
-        <v>290</v>
+        <v>602</v>
       </c>
     </row>
     <row r="428" spans="1:4">
@@ -8855,7 +8886,7 @@
         <v>603</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C428" s="4" t="s">
         <v>6</v>
@@ -8869,7 +8900,7 @@
         <v>603</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C429" s="4" t="s">
         <v>6</v>
@@ -8880,16 +8911,16 @@
     </row>
     <row r="430" spans="1:4">
       <c r="A430" s="2" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C430" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D430" s="5" t="s">
-        <v>609</v>
+        <v>290</v>
       </c>
     </row>
     <row r="431" spans="1:4">
@@ -8897,7 +8928,7 @@
         <v>607</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C431" s="4" t="s">
         <v>6</v>
@@ -8911,7 +8942,7 @@
         <v>607</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C432" s="4" t="s">
         <v>6</v>
@@ -8925,7 +8956,7 @@
         <v>607</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C433" s="4" t="s">
         <v>6</v>
@@ -8936,16 +8967,16 @@
     </row>
     <row r="434" spans="1:4">
       <c r="A434" s="2" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C434" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D434" s="5" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
     </row>
     <row r="435" spans="1:4">
@@ -8953,7 +8984,7 @@
         <v>613</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C435" s="4" t="s">
         <v>6</v>
@@ -8967,7 +8998,7 @@
         <v>613</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>6</v>
@@ -8978,16 +9009,16 @@
     </row>
     <row r="437" spans="1:4">
       <c r="A437" s="2" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D437" s="5" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
     </row>
     <row r="438" spans="1:4">
@@ -8995,7 +9026,7 @@
         <v>618</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>6</v>
@@ -9009,7 +9040,7 @@
         <v>618</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>6</v>
@@ -9023,7 +9054,7 @@
         <v>618</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>6</v>
@@ -9034,16 +9065,16 @@
     </row>
     <row r="441" spans="1:4">
       <c r="A441" s="2" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D441" s="5" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="442" spans="1:4">
@@ -9051,7 +9082,7 @@
         <v>624</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>6</v>
@@ -9065,7 +9096,7 @@
         <v>624</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>6</v>
@@ -9079,7 +9110,7 @@
         <v>624</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C444" s="4" t="s">
         <v>6</v>
@@ -9090,16 +9121,16 @@
     </row>
     <row r="445" spans="1:4">
       <c r="A445" s="2" t="s">
-        <v>76</v>
+        <v>624</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D445" s="5" t="s">
-        <v>78</v>
+        <v>626</v>
       </c>
     </row>
     <row r="446" spans="1:4">
@@ -9107,7 +9138,7 @@
         <v>76</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>6</v>
@@ -9121,7 +9152,7 @@
         <v>76</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>6</v>
@@ -9132,16 +9163,16 @@
     </row>
     <row r="448" spans="1:4">
       <c r="A448" s="2" t="s">
-        <v>633</v>
+        <v>76</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D448" s="5" t="s">
-        <v>635</v>
+        <v>78</v>
       </c>
     </row>
     <row r="449" spans="1:4">
@@ -9149,7 +9180,7 @@
         <v>633</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>6</v>
@@ -9163,7 +9194,7 @@
         <v>633</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>6</v>
@@ -9177,7 +9208,7 @@
         <v>633</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>6</v>
@@ -9188,16 +9219,16 @@
     </row>
     <row r="452" spans="1:4">
       <c r="A452" s="2" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D452" s="5" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
     </row>
     <row r="453" spans="1:4">
@@ -9205,7 +9236,7 @@
         <v>639</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>6</v>
@@ -9219,7 +9250,7 @@
         <v>639</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>6</v>
@@ -9230,44 +9261,44 @@
     </row>
     <row r="455" spans="1:4">
       <c r="A455" s="2" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D455" s="5" t="s">
-        <v>54</v>
+        <v>641</v>
       </c>
     </row>
     <row r="456" spans="1:4">
       <c r="A456" s="2" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D456" s="5" t="s">
-        <v>648</v>
+        <v>54</v>
       </c>
     </row>
     <row r="457" spans="1:4">
       <c r="A457" s="2" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D457" s="5" t="s">
-        <v>125</v>
+        <v>648</v>
       </c>
     </row>
     <row r="458" spans="1:4">
@@ -9275,7 +9306,7 @@
         <v>649</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>6</v>
@@ -9289,7 +9320,7 @@
         <v>649</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>6</v>
@@ -9300,16 +9331,16 @@
     </row>
     <row r="460" spans="1:4">
       <c r="A460" s="2" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D460" s="5" t="s">
-        <v>814</v>
+        <v>125</v>
       </c>
     </row>
     <row r="461" spans="1:4">
@@ -9317,7 +9348,7 @@
         <v>653</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>6</v>
@@ -9331,7 +9362,7 @@
         <v>653</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>6</v>
@@ -9345,7 +9376,7 @@
         <v>653</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>6</v>
@@ -9359,7 +9390,7 @@
         <v>653</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>6</v>
@@ -9370,16 +9401,16 @@
     </row>
     <row r="465" spans="1:4">
       <c r="A465" s="2" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D465" s="5" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
     <row r="466" spans="1:4">
@@ -9387,7 +9418,7 @@
         <v>659</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>6</v>
@@ -9401,7 +9432,7 @@
         <v>659</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>6</v>
@@ -9412,16 +9443,16 @@
     </row>
     <row r="468" spans="1:4">
       <c r="A468" s="2" t="s">
-        <v>288</v>
+        <v>659</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D468" s="5" t="s">
-        <v>290</v>
+        <v>812</v>
       </c>
     </row>
     <row r="469" spans="1:4">
@@ -9429,7 +9460,7 @@
         <v>288</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>6</v>
@@ -9443,7 +9474,7 @@
         <v>288</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C470" s="4" t="s">
         <v>6</v>
@@ -9454,16 +9485,16 @@
     </row>
     <row r="471" spans="1:4">
       <c r="A471" s="2" t="s">
-        <v>64</v>
+        <v>288</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C471" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D471" s="5" t="s">
-        <v>7</v>
+        <v>290</v>
       </c>
     </row>
     <row r="472" spans="1:4">
@@ -9471,7 +9502,7 @@
         <v>64</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C472" s="4" t="s">
         <v>6</v>
@@ -9482,16 +9513,16 @@
     </row>
     <row r="473" spans="1:4">
       <c r="A473" s="2" t="s">
-        <v>668</v>
+        <v>64</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C473" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D473" s="5" t="s">
-        <v>648</v>
+        <v>7</v>
       </c>
     </row>
     <row r="474" spans="1:4">
@@ -9499,7 +9530,7 @@
         <v>668</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>6</v>
@@ -9513,7 +9544,7 @@
         <v>668</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>6</v>
@@ -9524,16 +9555,16 @@
     </row>
     <row r="476" spans="1:4">
       <c r="A476" s="2" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D476" s="5" t="s">
-        <v>125</v>
+        <v>648</v>
       </c>
     </row>
     <row r="477" spans="1:4">
@@ -9541,7 +9572,7 @@
         <v>672</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>6</v>
@@ -9552,16 +9583,16 @@
     </row>
     <row r="478" spans="1:4">
       <c r="A478" s="2" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D478" s="5" t="s">
-        <v>677</v>
+        <v>125</v>
       </c>
     </row>
     <row r="479" spans="1:4">
@@ -9569,7 +9600,7 @@
         <v>675</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>6</v>
@@ -9583,7 +9614,7 @@
         <v>675</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C480" s="4" t="s">
         <v>6</v>
@@ -9594,16 +9625,16 @@
     </row>
     <row r="481" spans="1:4">
       <c r="A481" s="2" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C481" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D481" s="5" t="s">
-        <v>54</v>
+        <v>677</v>
       </c>
     </row>
     <row r="482" spans="1:4">
@@ -9611,7 +9642,7 @@
         <v>680</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C482" s="4" t="s">
         <v>6</v>
@@ -9625,7 +9656,7 @@
         <v>680</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C483" s="4" t="s">
         <v>6</v>
@@ -9636,30 +9667,30 @@
     </row>
     <row r="484" spans="1:4">
       <c r="A484" s="2" t="s">
-        <v>553</v>
+        <v>680</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C484" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D484" s="5" t="s">
-        <v>555</v>
+        <v>54</v>
       </c>
     </row>
     <row r="485" spans="1:4">
       <c r="A485" s="2" t="s">
-        <v>685</v>
+        <v>553</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C485" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D485" s="5" t="s">
-        <v>68</v>
+        <v>555</v>
       </c>
     </row>
     <row r="486" spans="1:4">
@@ -9667,7 +9698,7 @@
         <v>685</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C486" s="4" t="s">
         <v>6</v>
@@ -9681,7 +9712,7 @@
         <v>685</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C487" s="4" t="s">
         <v>6</v>
@@ -9695,7 +9726,7 @@
         <v>685</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C488" s="4" t="s">
         <v>6</v>
@@ -9709,7 +9740,7 @@
         <v>685</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C489" s="4" t="s">
         <v>6</v>
@@ -9720,44 +9751,44 @@
     </row>
     <row r="490" spans="1:4">
       <c r="A490" s="2" t="s">
-        <v>558</v>
+        <v>685</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C490" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D490" s="5" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
     </row>
     <row r="491" spans="1:4">
       <c r="A491" s="2" t="s">
-        <v>575</v>
+        <v>558</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C491" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D491" s="5" t="s">
-        <v>577</v>
+        <v>125</v>
       </c>
     </row>
     <row r="492" spans="1:4">
       <c r="A492" s="2" t="s">
-        <v>693</v>
+        <v>575</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C492" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D492" s="5" t="s">
-        <v>466</v>
+        <v>577</v>
       </c>
     </row>
     <row r="493" spans="1:4">
@@ -9765,7 +9796,7 @@
         <v>693</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C493" s="4" t="s">
         <v>6</v>
@@ -9779,7 +9810,7 @@
         <v>693</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C494" s="4" t="s">
         <v>6</v>
@@ -9790,30 +9821,30 @@
     </row>
     <row r="495" spans="1:4">
       <c r="A495" s="2" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C495" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D495" s="5" t="s">
-        <v>296</v>
+        <v>466</v>
       </c>
     </row>
     <row r="496" spans="1:4">
       <c r="A496" s="2" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B496" s="3" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C496" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D496" s="5" t="s">
-        <v>701</v>
+        <v>296</v>
       </c>
     </row>
     <row r="497" spans="1:4">
@@ -9821,7 +9852,7 @@
         <v>699</v>
       </c>
       <c r="B497" s="3" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C497" s="4" t="s">
         <v>6</v>
@@ -9835,7 +9866,7 @@
         <v>699</v>
       </c>
       <c r="B498" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C498" s="4" t="s">
         <v>6</v>
@@ -9846,30 +9877,30 @@
     </row>
     <row r="499" spans="1:4">
       <c r="A499" s="2" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="B499" s="3" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C499" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D499" s="5" t="s">
-        <v>620</v>
+        <v>701</v>
       </c>
     </row>
     <row r="500" spans="1:4">
       <c r="A500" s="2" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B500" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C500" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D500" s="5" t="s">
-        <v>708</v>
+        <v>620</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -9877,7 +9908,7 @@
         <v>706</v>
       </c>
       <c r="B501" s="3" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C501" s="4" t="s">
         <v>6</v>
@@ -9888,30 +9919,30 @@
     </row>
     <row r="502" spans="1:4">
       <c r="A502" s="2" t="s">
-        <v>693</v>
+        <v>706</v>
       </c>
       <c r="B502" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C502" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D502" s="5" t="s">
-        <v>466</v>
+        <v>708</v>
       </c>
     </row>
     <row r="503" spans="1:4">
       <c r="A503" s="2" t="s">
-        <v>711</v>
+        <v>693</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C503" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D503" s="5" t="s">
-        <v>10</v>
+        <v>466</v>
       </c>
     </row>
     <row r="504" spans="1:4">
@@ -9919,7 +9950,7 @@
         <v>711</v>
       </c>
       <c r="B504" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C504" s="4" t="s">
         <v>6</v>
@@ -9933,7 +9964,7 @@
         <v>711</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C505" s="4" t="s">
         <v>6</v>
@@ -9947,7 +9978,7 @@
         <v>711</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C506" s="4" t="s">
         <v>6</v>
@@ -9958,16 +9989,16 @@
     </row>
     <row r="507" spans="1:4">
       <c r="A507" s="2" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="B507" s="3" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C507" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D507" s="5" t="s">
-        <v>555</v>
+        <v>10</v>
       </c>
     </row>
     <row r="508" spans="1:4">
@@ -9975,7 +10006,7 @@
         <v>716</v>
       </c>
       <c r="B508" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C508" s="4" t="s">
         <v>6</v>
@@ -9989,7 +10020,7 @@
         <v>716</v>
       </c>
       <c r="B509" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C509" s="4" t="s">
         <v>6</v>
@@ -10000,16 +10031,16 @@
     </row>
     <row r="510" spans="1:4">
       <c r="A510" s="2" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C510" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D510" s="5" t="s">
-        <v>125</v>
+        <v>555</v>
       </c>
     </row>
     <row r="511" spans="1:4">
@@ -10017,7 +10048,7 @@
         <v>720</v>
       </c>
       <c r="B511" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C511" s="4" t="s">
         <v>6</v>
@@ -10031,7 +10062,7 @@
         <v>720</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C512" s="4" t="s">
         <v>6</v>
@@ -10042,30 +10073,30 @@
     </row>
     <row r="513" spans="1:4">
       <c r="A513" s="2" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C513" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D513" s="5" t="s">
-        <v>577</v>
+        <v>125</v>
       </c>
     </row>
     <row r="514" spans="1:4">
       <c r="A514" s="2" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B514" s="3" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C514" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D514" s="5" t="s">
-        <v>728</v>
+        <v>577</v>
       </c>
     </row>
     <row r="515" spans="1:4">
@@ -10073,7 +10104,7 @@
         <v>726</v>
       </c>
       <c r="B515" s="3" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C515" s="4" t="s">
         <v>6</v>
@@ -10087,7 +10118,7 @@
         <v>726</v>
       </c>
       <c r="B516" s="3" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C516" s="4" t="s">
         <v>6</v>
@@ -10098,16 +10129,16 @@
     </row>
     <row r="517" spans="1:4">
       <c r="A517" s="2" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="B517" s="3" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C517" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D517" s="5" t="s">
-        <v>319</v>
+        <v>728</v>
       </c>
     </row>
     <row r="518" spans="1:4">
@@ -10115,7 +10146,7 @@
         <v>731</v>
       </c>
       <c r="B518" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C518" s="4" t="s">
         <v>6</v>
@@ -10126,16 +10157,16 @@
     </row>
     <row r="519" spans="1:4">
       <c r="A519" s="2" t="s">
-        <v>196</v>
+        <v>731</v>
       </c>
       <c r="B519" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C519" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D519" s="5" t="s">
-        <v>198</v>
+        <v>319</v>
       </c>
     </row>
     <row r="520" spans="1:4">
@@ -10143,7 +10174,7 @@
         <v>196</v>
       </c>
       <c r="B520" s="3" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C520" s="4" t="s">
         <v>6</v>
@@ -10157,7 +10188,7 @@
         <v>196</v>
       </c>
       <c r="B521" s="3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C521" s="4" t="s">
         <v>6</v>
@@ -10168,16 +10199,16 @@
     </row>
     <row r="522" spans="1:4">
       <c r="A522" s="2" t="s">
-        <v>302</v>
+        <v>196</v>
       </c>
       <c r="B522" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C522" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D522" s="5" t="s">
-        <v>304</v>
+        <v>198</v>
       </c>
     </row>
     <row r="523" spans="1:4">
@@ -10185,7 +10216,7 @@
         <v>302</v>
       </c>
       <c r="B523" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C523" s="4" t="s">
         <v>6</v>
@@ -10199,7 +10230,7 @@
         <v>302</v>
       </c>
       <c r="B524" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C524" s="4" t="s">
         <v>6</v>
@@ -10210,44 +10241,44 @@
     </row>
     <row r="525" spans="1:4">
       <c r="A525" s="2" t="s">
-        <v>740</v>
+        <v>302</v>
       </c>
       <c r="B525" s="3" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C525" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D525" s="5" t="s">
-        <v>366</v>
+        <v>304</v>
       </c>
     </row>
     <row r="526" spans="1:4">
       <c r="A526" s="2" t="s">
-        <v>302</v>
+        <v>740</v>
       </c>
       <c r="B526" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C526" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D526" s="5" t="s">
-        <v>304</v>
+        <v>366</v>
       </c>
     </row>
     <row r="527" spans="1:4">
       <c r="A527" s="2" t="s">
-        <v>740</v>
+        <v>302</v>
       </c>
       <c r="B527" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C527" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D527" s="5" t="s">
-        <v>366</v>
+        <v>304</v>
       </c>
     </row>
     <row r="528" spans="1:4">
@@ -10255,7 +10286,7 @@
         <v>740</v>
       </c>
       <c r="B528" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C528" s="4" t="s">
         <v>6</v>
@@ -10266,16 +10297,16 @@
     </row>
     <row r="529" spans="1:4">
       <c r="A529" s="2" t="s">
-        <v>302</v>
+        <v>740</v>
       </c>
       <c r="B529" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C529" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D529" s="5" t="s">
-        <v>304</v>
+        <v>366</v>
       </c>
     </row>
     <row r="530" spans="1:4">
@@ -10283,7 +10314,7 @@
         <v>302</v>
       </c>
       <c r="B530" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C530" s="4" t="s">
         <v>6</v>
@@ -10297,7 +10328,7 @@
         <v>302</v>
       </c>
       <c r="B531" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C531" s="4" t="s">
         <v>6</v>
@@ -10308,30 +10339,30 @@
     </row>
     <row r="532" spans="1:4">
       <c r="A532" s="2" t="s">
-        <v>748</v>
+        <v>302</v>
       </c>
       <c r="B532" s="3" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C532" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D532" s="5" t="s">
-        <v>750</v>
+        <v>304</v>
       </c>
     </row>
     <row r="533" spans="1:4">
       <c r="A533" s="2" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="B533" s="3" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="C533" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D533" s="5" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="534" spans="1:4">
@@ -10339,7 +10370,7 @@
         <v>751</v>
       </c>
       <c r="B534" s="3" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C534" s="4" t="s">
         <v>6</v>
@@ -10353,7 +10384,7 @@
         <v>751</v>
       </c>
       <c r="B535" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C535" s="4" t="s">
         <v>6</v>
@@ -10364,30 +10395,30 @@
     </row>
     <row r="536" spans="1:4">
       <c r="A536" s="2" t="s">
-        <v>731</v>
+        <v>751</v>
       </c>
       <c r="B536" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C536" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D536" s="5" t="s">
-        <v>319</v>
+        <v>753</v>
       </c>
     </row>
     <row r="537" spans="1:4">
       <c r="A537" s="2" t="s">
-        <v>697</v>
+        <v>731</v>
       </c>
       <c r="B537" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C537" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D537" s="5" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
     </row>
     <row r="538" spans="1:4">
@@ -10395,7 +10426,7 @@
         <v>697</v>
       </c>
       <c r="B538" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C538" s="4" t="s">
         <v>6</v>
@@ -10406,44 +10437,44 @@
     </row>
     <row r="539" spans="1:4">
       <c r="A539" s="2" t="s">
-        <v>731</v>
+        <v>697</v>
       </c>
       <c r="B539" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C539" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D539" s="5" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
     </row>
     <row r="540" spans="1:4">
       <c r="A540" s="2" t="s">
-        <v>697</v>
+        <v>731</v>
       </c>
       <c r="B540" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C540" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D540" s="5" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
     </row>
     <row r="541" spans="1:4">
       <c r="A541" s="2" t="s">
-        <v>731</v>
+        <v>697</v>
       </c>
       <c r="B541" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C541" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D541" s="5" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
     </row>
     <row r="542" spans="1:4">
@@ -10451,7 +10482,7 @@
         <v>731</v>
       </c>
       <c r="B542" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C542" s="4" t="s">
         <v>6</v>
@@ -10462,16 +10493,16 @@
     </row>
     <row r="543" spans="1:4">
       <c r="A543" s="2" t="s">
-        <v>763</v>
+        <v>731</v>
       </c>
       <c r="B543" s="3" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C543" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D543" s="5" t="s">
-        <v>750</v>
+        <v>319</v>
       </c>
     </row>
     <row r="544" spans="1:4">
@@ -10479,7 +10510,7 @@
         <v>763</v>
       </c>
       <c r="B544" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C544" s="4" t="s">
         <v>6</v>
@@ -10493,7 +10524,7 @@
         <v>763</v>
       </c>
       <c r="B545" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C545" s="4" t="s">
         <v>6</v>
@@ -10504,16 +10535,16 @@
     </row>
     <row r="546" spans="1:4">
       <c r="A546" s="2" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="B546" s="3" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C546" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D546" s="5" t="s">
-        <v>198</v>
+        <v>750</v>
       </c>
     </row>
     <row r="547" spans="1:4">
@@ -10521,7 +10552,7 @@
         <v>767</v>
       </c>
       <c r="B547" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C547" s="4" t="s">
         <v>6</v>
@@ -10535,7 +10566,7 @@
         <v>767</v>
       </c>
       <c r="B548" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C548" s="4" t="s">
         <v>6</v>
@@ -10549,7 +10580,7 @@
         <v>767</v>
       </c>
       <c r="B549" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C549" s="4" t="s">
         <v>6</v>
@@ -10560,16 +10591,16 @@
     </row>
     <row r="550" spans="1:4">
       <c r="A550" s="2" t="s">
-        <v>294</v>
+        <v>767</v>
       </c>
       <c r="B550" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C550" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D550" s="5" t="s">
-        <v>296</v>
+        <v>198</v>
       </c>
     </row>
     <row r="551" spans="1:4">
@@ -10577,7 +10608,7 @@
         <v>294</v>
       </c>
       <c r="B551" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C551" s="4" t="s">
         <v>6</v>
@@ -10591,7 +10622,7 @@
         <v>294</v>
       </c>
       <c r="B552" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C552" s="4" t="s">
         <v>6</v>
@@ -10605,7 +10636,7 @@
         <v>294</v>
       </c>
       <c r="B553" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C553" s="4" t="s">
         <v>6</v>
@@ -10619,7 +10650,7 @@
         <v>294</v>
       </c>
       <c r="B554" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C554" s="4" t="s">
         <v>6</v>
@@ -10630,58 +10661,58 @@
     </row>
     <row r="555" spans="1:4">
       <c r="A555" s="2" t="s">
-        <v>196</v>
+        <v>294</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C555" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D555" s="5" t="s">
-        <v>198</v>
+        <v>296</v>
       </c>
     </row>
     <row r="556" spans="1:4">
       <c r="A556" s="2" t="s">
-        <v>294</v>
+        <v>196</v>
       </c>
       <c r="B556" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C556" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D556" s="5" t="s">
-        <v>296</v>
+        <v>198</v>
       </c>
     </row>
     <row r="557" spans="1:4">
       <c r="A557" s="2" t="s">
-        <v>196</v>
+        <v>294</v>
       </c>
       <c r="B557" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C557" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D557" s="5" t="s">
-        <v>198</v>
+        <v>296</v>
       </c>
     </row>
     <row r="558" spans="1:4">
       <c r="A558" s="2" t="s">
-        <v>780</v>
+        <v>196</v>
       </c>
       <c r="B558" s="3" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C558" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D558" s="5" t="s">
-        <v>648</v>
+        <v>198</v>
       </c>
     </row>
     <row r="559" spans="1:4">
@@ -10689,7 +10720,7 @@
         <v>780</v>
       </c>
       <c r="B559" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C559" s="4" t="s">
         <v>6</v>
@@ -10700,44 +10731,44 @@
     </row>
     <row r="560" spans="1:4">
       <c r="A560" s="2" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="B560" s="3" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C560" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D560" s="5" t="s">
-        <v>750</v>
+        <v>648</v>
       </c>
     </row>
     <row r="561" spans="1:4">
       <c r="A561" s="2" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="B561" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C561" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D561" s="5" t="s">
-        <v>648</v>
+        <v>750</v>
       </c>
     </row>
     <row r="562" spans="1:4">
       <c r="A562" s="2" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="B562" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C562" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D562" s="5" t="s">
-        <v>750</v>
+        <v>648</v>
       </c>
     </row>
     <row r="563" spans="1:4">
@@ -10745,7 +10776,7 @@
         <v>783</v>
       </c>
       <c r="B563" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C563" s="4" t="s">
         <v>6</v>
@@ -10756,44 +10787,44 @@
     </row>
     <row r="564" spans="1:4">
       <c r="A564" s="2" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="B564" s="3" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C564" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D564" s="5" t="s">
-        <v>790</v>
+        <v>750</v>
       </c>
     </row>
     <row r="565" spans="1:4">
       <c r="A565" s="2" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="B565" s="3" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C565" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D565" s="5" t="s">
-        <v>90</v>
+        <v>790</v>
       </c>
     </row>
     <row r="566" spans="1:4">
       <c r="A566" s="2" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B566" s="3" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C566" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D566" s="5" t="s">
-        <v>466</v>
+        <v>90</v>
       </c>
     </row>
     <row r="567" spans="1:4">
@@ -10801,7 +10832,7 @@
         <v>793</v>
       </c>
       <c r="B567" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C567" s="4" t="s">
         <v>6</v>
@@ -10815,7 +10846,7 @@
         <v>793</v>
       </c>
       <c r="B568" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C568" s="4" t="s">
         <v>6</v>
@@ -10826,10 +10857,10 @@
     </row>
     <row r="569" spans="1:4">
       <c r="A569" s="2" t="s">
-        <v>693</v>
+        <v>793</v>
       </c>
       <c r="B569" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C569" s="4" t="s">
         <v>6</v>
@@ -10843,7 +10874,7 @@
         <v>693</v>
       </c>
       <c r="B570" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C570" s="4" t="s">
         <v>6</v>
@@ -10854,10 +10885,10 @@
     </row>
     <row r="571" spans="1:4">
       <c r="A571" s="2" t="s">
-        <v>793</v>
+        <v>693</v>
       </c>
       <c r="B571" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C571" s="4" t="s">
         <v>6</v>
@@ -10868,10 +10899,10 @@
     </row>
     <row r="572" spans="1:4">
       <c r="A572" s="2" t="s">
-        <v>693</v>
+        <v>793</v>
       </c>
       <c r="B572" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C572" s="4" t="s">
         <v>6</v>
@@ -10882,30 +10913,30 @@
     </row>
     <row r="573" spans="1:4">
       <c r="A573" s="2" t="s">
-        <v>359</v>
+        <v>693</v>
       </c>
       <c r="B573" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C573" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D573" s="5" t="s">
-        <v>13</v>
+        <v>466</v>
       </c>
     </row>
     <row r="574" spans="1:4">
       <c r="A574" s="2" t="s">
-        <v>693</v>
+        <v>359</v>
       </c>
       <c r="B574" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C574" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D574" s="5" t="s">
-        <v>466</v>
+        <v>13</v>
       </c>
     </row>
     <row r="575" spans="1:4">
@@ -10913,7 +10944,7 @@
         <v>693</v>
       </c>
       <c r="B575" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C575" s="4" t="s">
         <v>6</v>
@@ -10924,16 +10955,16 @@
     </row>
     <row r="576" spans="1:4">
       <c r="A576" s="2" t="s">
-        <v>600</v>
+        <v>693</v>
       </c>
       <c r="B576" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C576" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D576" s="5" t="s">
-        <v>602</v>
+        <v>466</v>
       </c>
     </row>
     <row r="577" spans="1:4">
@@ -10941,7 +10972,7 @@
         <v>600</v>
       </c>
       <c r="B577" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C577" s="4" t="s">
         <v>6</v>
@@ -10952,16 +10983,16 @@
     </row>
     <row r="578" spans="1:4">
       <c r="A578" s="2" t="s">
-        <v>806</v>
+        <v>600</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C578" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D578" s="5" t="s">
-        <v>808</v>
+        <v>602</v>
       </c>
     </row>
     <row r="579" spans="1:4">
@@ -10969,7 +11000,7 @@
         <v>806</v>
       </c>
       <c r="B579" s="3" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C579" s="4" t="s">
         <v>6</v>
@@ -10983,7 +11014,7 @@
         <v>806</v>
       </c>
       <c r="B580" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C580" s="4" t="s">
         <v>6</v>
@@ -10993,21 +11024,36 @@
       </c>
     </row>
     <row r="581" spans="1:4">
-      <c r="A581" t="s">
+      <c r="A581" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="B581" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="C581" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D581" s="5" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="582" spans="1:4">
+      <c r="A582" t="s">
         <v>150</v>
       </c>
-      <c r="B581" t="s">
+      <c r="B582" t="s">
         <v>811</v>
       </c>
-      <c r="C581" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D581" s="6">
+      <c r="C582" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D582" s="6">
         <v>141</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>